<commit_message>
map edf remove ore
</commit_message>
<xml_diff>
--- a/gu_in/Map.edf/neutralAS1.xlsx
+++ b/gu_in/Map.edf/neutralAS1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\emay.dev\Parser_1.0.2\Database\gu_in\Map.edf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD688AF0-E2FA-410A-B430-80E6D907CA94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83E3BB19-5C98-4ECE-8CF8-0355418468AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1125" yWindow="1125" windowWidth="18480" windowHeight="11205" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38283,7 +38283,7 @@
   <dimension ref="A1:H90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -38351,7 +38351,7 @@
         <v>9220</v>
       </c>
       <c r="D3" s="1">
-        <v>772</v>
+        <v>200772</v>
       </c>
       <c r="E3" s="1">
         <v>6826</v>
@@ -38455,7 +38455,7 @@
         <v>9146</v>
       </c>
       <c r="D7" s="1">
-        <v>776</v>
+        <v>200776</v>
       </c>
       <c r="E7" s="1">
         <v>6773</v>

</xml_diff>